<commit_message>
last version for the classification
</commit_message>
<xml_diff>
--- a/_PETRO/MALI_counts.xlsx
+++ b/_PETRO/MALI_counts.xlsx
@@ -390,7 +390,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1459</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="4">
@@ -410,7 +410,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>